<commit_message>
creating cases to test sets default to PRE/NRG for process/commodity, when not specified on the top of process/commodity tables
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs-SolWin.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs-SolWin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FFA9D0B-85B2-44F4-85FA-AF48C5B92220}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0D130-3FB9-4E41-A707-8233BE3EB869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27285" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_SolWin" sheetId="4" r:id="rId1"/>
@@ -21,20 +21,12 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t>~FI_T</t>
   </si>
@@ -325,16 +317,22 @@
   </si>
   <si>
     <t>Power Plants New 2 - Solar energy</t>
+  </si>
+  <si>
+    <t>dumcom_sets</t>
+  </si>
+  <si>
+    <t>commodity to test sets defaulting to NRG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="214" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -623,14 +621,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -756,86 +754,86 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="214" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="214" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="214" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="214" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="214" fontId="20" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="214" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="214" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="214" fontId="11" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="214" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="15" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="15" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
-    <cellStyle name="calculated" xfId="3"/>
-    <cellStyle name="Calculation 2" xfId="4"/>
-    <cellStyle name="Comma 10" xfId="5"/>
-    <cellStyle name="Comma 11" xfId="6"/>
-    <cellStyle name="Comma 2" xfId="7"/>
-    <cellStyle name="Comma 2 2" xfId="8"/>
-    <cellStyle name="Comma 2 3" xfId="9"/>
-    <cellStyle name="Comma 2 4" xfId="10"/>
-    <cellStyle name="Comma 2 5" xfId="11"/>
-    <cellStyle name="Comma 3" xfId="12"/>
+    <cellStyle name="calculated" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Calculation 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 10" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 11" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Comma 2 5" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Comma 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Good" xfId="13" builtinId="26"/>
-    <cellStyle name="Hyperlink 3" xfId="14"/>
+    <cellStyle name="Hyperlink 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="15"/>
-    <cellStyle name="Normal 11" xfId="16"/>
-    <cellStyle name="Normal 11 2" xfId="17"/>
-    <cellStyle name="Normal 11 3" xfId="18"/>
-    <cellStyle name="Normal 11 4" xfId="19"/>
-    <cellStyle name="Normal 12" xfId="20"/>
-    <cellStyle name="Normal 12 2" xfId="21"/>
-    <cellStyle name="Normal 12 3" xfId="22"/>
-    <cellStyle name="Normal 12 4" xfId="23"/>
-    <cellStyle name="Normal 2" xfId="24"/>
-    <cellStyle name="Normal 2 2" xfId="25"/>
-    <cellStyle name="Normal 2 3" xfId="26"/>
-    <cellStyle name="Normal 2 4" xfId="27"/>
-    <cellStyle name="Normal 3" xfId="28"/>
-    <cellStyle name="Normal 39" xfId="29"/>
-    <cellStyle name="Normal 4" xfId="30"/>
-    <cellStyle name="Normal 4 2" xfId="31"/>
-    <cellStyle name="Normal 8" xfId="32"/>
-    <cellStyle name="Normal 9 2" xfId="33"/>
-    <cellStyle name="Normale_B2020" xfId="34"/>
-    <cellStyle name="Note 2" xfId="35"/>
-    <cellStyle name="Percent 2" xfId="36"/>
-    <cellStyle name="Percent 2 2" xfId="37"/>
-    <cellStyle name="Percent 2 2 2" xfId="38"/>
-    <cellStyle name="Percent 2 3" xfId="39"/>
-    <cellStyle name="Percent 3" xfId="40"/>
-    <cellStyle name="Percent 3 2" xfId="41"/>
-    <cellStyle name="Percent 3 2 2" xfId="42"/>
-    <cellStyle name="Percent 3 3" xfId="43"/>
-    <cellStyle name="Percent 3 4" xfId="44"/>
-    <cellStyle name="Percent 4" xfId="45"/>
-    <cellStyle name="Percent 4 2" xfId="46"/>
-    <cellStyle name="Percent 4 3" xfId="47"/>
-    <cellStyle name="Percent 4 4" xfId="48"/>
-    <cellStyle name="Percent 5" xfId="49"/>
-    <cellStyle name="Percent 5 2" xfId="50"/>
-    <cellStyle name="Percent 6" xfId="51"/>
-    <cellStyle name="Percent 6 2" xfId="52"/>
-    <cellStyle name="Percent 7" xfId="53"/>
-    <cellStyle name="Percent 8" xfId="54"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="55"/>
+    <cellStyle name="Normal 10" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 11" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 11 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 11 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 11 4" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 12" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 12 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 12 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 12 4" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 2 3" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 2 4" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 39" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 4" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 8" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 9 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normale_B2020" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Note 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Percent 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Percent 2 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Percent 2 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Percent 2 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Percent 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Percent 3 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Percent 3 2 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Percent 3 3" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Percent 3 4" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Percent 4" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Percent 4 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Percent 4 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Percent 4 4" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Percent 5" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Percent 5 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Percent 6" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Percent 6 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Percent 7" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Percent 8" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1535,12 +1533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1751,9 +1749,15 @@
       <c r="O7" s="22"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
+      <c r="R7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>

</xml_diff>

<commit_message>
introducing a scen file for GAMS commands example; creating commodity-only attributes case in SubRES
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs-SolWin.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs-SolWin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0D130-3FB9-4E41-A707-8233BE3EB869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEBB9DC-59CA-4874-AA5D-2A9D5F39AD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27285" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1530" windowWidth="13755" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_SolWin" sheetId="4" r:id="rId1"/>
@@ -21,12 +21,23 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
   <si>
     <t>~FI_T</t>
   </si>
@@ -323,6 +334,27 @@
   </si>
   <si>
     <t>commodity to test sets defaulting to NRG</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>ELCHYD</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>COM_BNDNET</t>
+  </si>
+  <si>
+    <t>~FI_T: COM_FR~LO</t>
+  </si>
+  <si>
+    <t>COM_TAXNET</t>
   </si>
 </sst>
 </file>
@@ -1537,8 +1569,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2297,10 +2329,62 @@
       <c r="K29" s="27"/>
       <c r="N29" s="27"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E36" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="21">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D38" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="21">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="23"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="23"/>
     </row>
   </sheetData>

</xml_diff>